<commit_message>
- Fragebogen zu Prof-Interview - Aufgabenverteilungs-Excel erweitert
</commit_message>
<xml_diff>
--- a/00_Projektmanagement/Aufgabenverteilung.xlsx
+++ b/00_Projektmanagement/Aufgabenverteilung.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26408DD9-C9B3-4C5B-9453-18C757DC3FFC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A8B14E12-DE44-4AD4-BFE6-4B08D424FD2D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Aufgabe</t>
   </si>
@@ -53,6 +53,21 @@
   </si>
   <si>
     <t>7 Tage</t>
+  </si>
+  <si>
+    <t>Cuong, Konstantin, Simon</t>
+  </si>
+  <si>
+    <t>Linda, Carola</t>
+  </si>
+  <si>
+    <t>Interviews/ Fokusgruppen</t>
+  </si>
+  <si>
+    <t>Verstehen &amp; Festlegen des Nutzungskontexts: Studenten</t>
+  </si>
+  <si>
+    <t>Verstehen &amp; Festlegen des Nutzungskontexts: Professoren</t>
   </si>
 </sst>
 </file>
@@ -175,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -186,6 +201,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -469,17 +488,17 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -507,7 +526,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -527,27 +546,51 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="8">
+        <v>43434</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="8">
+        <v>43441</v>
+      </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="8">
+        <v>43434</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="8">
+        <v>43441</v>
+      </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -555,8 +598,8 @@
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -564,8 +607,8 @@
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -573,8 +616,8 @@
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -582,8 +625,8 @@
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -591,8 +634,8 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -600,8 +643,8 @@
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -609,8 +652,8 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -618,8 +661,8 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -627,8 +670,8 @@
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -636,8 +679,8 @@
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -645,8 +688,8 @@
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -654,8 +697,8 @@
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -663,8 +706,8 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -672,8 +715,8 @@
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -681,8 +724,8 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -690,8 +733,8 @@
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -699,8 +742,8 @@
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -709,6 +752,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added screenshots, updated projectmanagement
</commit_message>
<xml_diff>
--- a/00_Projektmanagement/Aufgabenverteilung.xlsx
+++ b/00_Projektmanagement/Aufgabenverteilung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\career\study\term6\human_computer_interactions\project_oth_app\00_Projektmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53966E59-8F27-4ACC-AA25-C0041B3DAD65}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D040F95-8069-4095-AF32-65A4FFEA7C45}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="32760" yWindow="32760" windowWidth="16380" windowHeight="8190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Aufgabe</t>
   </si>
@@ -109,12 +109,32 @@
   </si>
   <si>
     <t>Carola, Cuong, Konstantin, Linda, Simon (siehe ../Erarbeiten_der_Gestaltungsloesungen/Prototyping Verteilung</t>
+  </si>
+  <si>
+    <t>User-Testing</t>
+  </si>
+  <si>
+    <t>Professor - Carola, Linda, Simon
+Sekretariat - Carola, Linda
+Student - Cuong, Konstantin</t>
+  </si>
+  <si>
+    <t>Abschlusspräsentation</t>
+  </si>
+  <si>
+    <t>Abschlussbericht</t>
+  </si>
+  <si>
+    <t>Evaluierung und Überarbeitung Axure-Prototyp</t>
+  </si>
+  <si>
+    <t>Carola, Cuong, Konstantin, Linda, Simon (siehe ../05_Abschlusspräsentation/Aufteilung wer macht was.docx)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
@@ -180,7 +200,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Excel Built-in Normal" xfId="1"/>
+    <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -645,11 +665,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,26 +890,42 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="5"/>
+    <row r="16" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="5"/>
+      <c r="D16" s="7">
+        <v>43480</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="5"/>
+    <row r="18" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>

</xml_diff>

<commit_message>
updated projectmanagement, deleted unused templates, updated Abschlussbericht
</commit_message>
<xml_diff>
--- a/00_Projektmanagement/Aufgabenverteilung.xlsx
+++ b/00_Projektmanagement/Aufgabenverteilung.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carola\Desktop\OTH\HCI\HCI_OTH_APP\00_Projektmanagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\career\study\term6\human_computer_interactions\project_oth_app\00_Projektmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A8F906-825C-404B-9A37-0877527053AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87794F01-527A-47CD-9662-D5EFEA6651A0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="16380" windowHeight="8190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Aufgabe</t>
   </si>
@@ -28,39 +28,15 @@
     <t>Zuständige Personen</t>
   </si>
   <si>
-    <t>Termin_Start</t>
-  </si>
-  <si>
-    <t>Termin_Ende</t>
-  </si>
-  <si>
-    <t>Analyse der aktuellen OTH Ersti-App</t>
-  </si>
-  <si>
-    <t>Carola, Cuong, Konstantin, Linda, Simon</t>
-  </si>
-  <si>
-    <t>Start und Verwaltung von git-repository und des Projektmanagement Ordners</t>
-  </si>
-  <si>
     <t>Simon</t>
   </si>
   <si>
-    <t>Enddate</t>
-  </si>
-  <si>
-    <t>Start und Verwaltung des Trello-Boards</t>
-  </si>
-  <si>
     <t>Carola</t>
   </si>
   <si>
     <t>Feature &amp; Stakeholder-Analyse</t>
   </si>
   <si>
-    <t>Studenten: Interviews, Szenarien</t>
-  </si>
-  <si>
     <t>Cuong, Konstantin, Simon</t>
   </si>
   <si>
@@ -88,26 +64,15 @@
     <t>Sketching</t>
   </si>
   <si>
-    <t>Start und Verwaltung des Axure-Share-Bereichs</t>
-  </si>
-  <si>
     <t>Cuong</t>
   </si>
   <si>
     <t>Axure-Prototyping</t>
   </si>
   <si>
-    <t>Carola, Cuong, Konstantin, Linda, Simon (siehe ../Erarbeiten_der_Gestaltungsloesungen/Prototyping Verteilung</t>
-  </si>
-  <si>
     <t>User-Testing</t>
   </si>
   <si>
-    <t>Professor - Carola, Linda, Simon
-Sekretariat - Carola, Linda
-Student - Cuong, Konstantin</t>
-  </si>
-  <si>
     <t>Abschlusspräsentation</t>
   </si>
   <si>
@@ -120,17 +85,63 @@
     <t>Interviews, Szenarien, Personas für Professoren, Sekretariat</t>
   </si>
   <si>
-    <t>Carola, Cuong, Linda, Simon (siehe ../05_Abschlusspräsentation/Aufteilung wer macht was.docx)</t>
+    <t>Analyse des aktuellen QIS-Systems</t>
+  </si>
+  <si>
+    <t>Management des git-Repository</t>
+  </si>
+  <si>
+    <t>Pflege des Projektmanagement-Ordners</t>
+  </si>
+  <si>
+    <t>Management des Trello-Boards</t>
+  </si>
+  <si>
+    <t>Management des Axure-Teamrepository</t>
+  </si>
+  <si>
+    <t>Alle</t>
+  </si>
+  <si>
+    <t>Interviews, Szenarien für Studenten</t>
+  </si>
+  <si>
+    <t>Erarbeitung: Alle, Erstellen des Dokuments: Carola, Linda</t>
+  </si>
+  <si>
+    <t>Erarbeitung: Alle, Erstellen des Dokuments: Carola</t>
+  </si>
+  <si>
+    <t>Carola, Linda: Dropdown Person/Druckerguthaben, Sekretariat-Oberfläche
+Cuong: Master Student/Professor/Sekretariat, Notenspiegel, Beitragsstatus, Immatrikulationsbescheinigung
+Konstantin: Kursanmeldung, Stundenplan, Prüfungsanmeldung
+Simon: Professoren-Oberfläche, Praktikumsstellen</t>
+  </si>
+  <si>
+    <t>Carola, Linda, Simon: Professor
+Carola, Linda: Sekretariat
+Cuong, Konstantin: Student</t>
+  </si>
+  <si>
+    <t>Carola: Verstehen und Festlegen des Nutzungskontext, Usability-Ergebnisse Sekretariat
+Cuong: Erarbeiten der Gestaltungslösungen, , Usability-Ergebnisse Student
+Konstantin: Endprodukt Highlight-Auswahl
+Linda: Festlegen der Nutzungsanforderungen
+Simon: Ausgangssituation, Usability-Ergebnisse Professoren</t>
+  </si>
+  <si>
+    <t>Carola: Verstehen und Festlegen des Nutzungskontext, Usability-Ergebnisse Sekretariat
+Cuong: Erarbeiten der Gestaltungslösungen, Usability-Ergebnisse Student
+Konstantin: Endprodukt Highlight-Auswahl
+Linda: Festlegen der Nutzungsanforderungen, Usability-Ergebnisse Sekretariat
+Simon: Projektinformationen, Projektmanagement, Ausgangssituation, Usability-Ergebnisse Professoren</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -152,7 +163,13 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -172,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -180,23 +197,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -665,305 +707,202 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="48.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B7" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4">
-        <v>43427</v>
-      </c>
-      <c r="D2" s="4">
-        <v>43434</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4">
-        <v>43427</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="B10" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B11" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B12" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4">
-        <v>43427</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="4">
-        <v>43434</v>
-      </c>
-      <c r="D5" s="4">
-        <v>43434</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B14" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4">
-        <v>43434</v>
-      </c>
-      <c r="D6" s="4">
-        <v>43441</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="B15" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="39" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="4">
-        <v>43434</v>
-      </c>
-      <c r="D7" s="4">
-        <v>43441</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="6">
-        <v>43441</v>
-      </c>
-      <c r="D8" s="6">
-        <v>43441</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="6">
-        <v>43441</v>
-      </c>
-      <c r="D9" s="6">
-        <v>43441</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    </row>
+    <row r="18" spans="1:2" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="6">
-        <v>43441</v>
-      </c>
-      <c r="D10" s="6">
-        <v>43441</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B19" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="6">
-        <v>43441</v>
-      </c>
-      <c r="D11" s="6">
-        <v>43441</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="6">
-        <v>43448</v>
-      </c>
-      <c r="D12" s="6">
-        <v>43448</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="6">
-        <v>43448</v>
-      </c>
-      <c r="D13" s="6">
-        <v>43454</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="7">
-        <v>43454</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="7">
-        <v>43454</v>
-      </c>
-      <c r="D15" s="7">
-        <v>43472</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="7">
-        <v>43480</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="B20" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>